<commit_message>
Doc de design pronto (ou quase)
Signed-off-by: Benito Michelon <benito@Benitos-MacBook-Pro.local>
</commit_message>
<xml_diff>
--- a/AuditoriaEq3byEq2.xlsx
+++ b/AuditoriaEq3byEq2.xlsx
@@ -1169,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1949,11 +1949,11 @@
         <v>9</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F37" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G37" s="28" t="s">
         <v>117</v>
@@ -1974,11 +1974,11 @@
         <v>8</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F38" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G38" s="28" t="s">
         <v>117</v>
@@ -1999,11 +1999,11 @@
         <v>9</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F39" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G39" s="28" t="s">
         <v>117</v>
@@ -2024,11 +2024,11 @@
         <v>8</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F40" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G40" s="28" t="s">
         <v>117</v>
@@ -2049,11 +2049,11 @@
         <v>7</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F41" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G41" s="28" t="s">
         <v>117</v>
@@ -2074,11 +2074,11 @@
         <v>7</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F42" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G42" s="28" t="s">
         <v>117</v>
@@ -2099,11 +2099,11 @@
         <v>7</v>
       </c>
       <c r="E43" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F43" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G43" s="28" t="s">
         <v>117</v>
@@ -2535,7 +2535,7 @@
       <c r="E61" s="20"/>
       <c r="F61" s="5">
         <f>SUM(F10:F60)</f>
-        <v>233</v>
+        <v>288</v>
       </c>
       <c r="G61" s="36"/>
     </row>
@@ -2550,7 +2550,7 @@
       <c r="E63" s="22"/>
       <c r="F63" s="17">
         <f>F61/D61*10</f>
-        <v>6.2466487935656829</v>
+        <v>7.7211796246648792</v>
       </c>
       <c r="G63" s="8" t="s">
         <v>5</v>
@@ -2613,7 +2613,7 @@
       </c>
       <c r="E70" s="24">
         <f>COUNTIF(E10:E60,"C")</f>
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -2625,7 +2625,7 @@
       </c>
       <c r="E71" s="24">
         <f>COUNTIF(E10:E60,"NC")</f>
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -2669,11 +2669,11 @@
       </c>
       <c r="E76" s="41">
         <f>SUM(F33:F43)</f>
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="F76" s="42">
         <f t="shared" si="9"/>
-        <v>1.625</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -2737,11 +2737,11 @@
       </c>
       <c r="E80" s="41">
         <f>SUM(E75:E79)</f>
-        <v>233</v>
+        <v>288</v>
       </c>
       <c r="F80" s="42">
         <f t="shared" si="9"/>
-        <v>6.2466487935656829</v>
+        <v>7.7211796246648792</v>
       </c>
     </row>
   </sheetData>

</xml_diff>